<commit_message>
Modificação nos gráficos do excel
</commit_message>
<xml_diff>
--- a/excel/analise_orcamentaria.xlsx
+++ b/excel/analise_orcamentaria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Desktop\Repositório\FP&amp;A\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CE1FFF-41D0-4520-972E-D3C1F5B6998D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E949CC8F-C7C0-42DB-862B-33D9DBA62221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="2" r:id="rId1"/>
@@ -2872,7 +2872,7 @@
         <c:axId val="1455861919"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="10000"/>
+          <c:min val="12000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2993,6 +2993,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -3040,6 +3071,7 @@
         <c14:dropZoneFilter val="1"/>
         <c14:dropZoneCategories val="1"/>
         <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
         <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
@@ -3090,9 +3122,10 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US"/>
               <a:t>Evolução do Realizado</a:t>
             </a:r>
+            <a:endParaRPr lang="en-US" baseline="0"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3235,6 +3268,9 @@
       <c:pivotFmt>
         <c:idx val="5"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3257,6 +3293,9 @@
       <c:pivotFmt>
         <c:idx val="6"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3279,6 +3318,9 @@
       <c:pivotFmt>
         <c:idx val="7"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3301,6 +3343,9 @@
       <c:pivotFmt>
         <c:idx val="8"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3323,6 +3368,9 @@
       <c:pivotFmt>
         <c:idx val="9"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -3369,7 +3417,7 @@
         <c:spPr>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -3391,7 +3439,7 @@
         <c:spPr>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -3413,6 +3461,116 @@
         <c:spPr>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="14"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="15"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="16"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="17"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="18"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
               <a:schemeClr val="accent4"/>
             </a:solidFill>
             <a:round/>
@@ -3431,7 +3589,7 @@
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="14"/>
+        <c:idx val="19"/>
         <c:spPr>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
@@ -3576,7 +3734,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000E-D463-402B-B436-56C38C4611DA}"/>
+              <c16:uniqueId val="{00000001-5211-4943-A1D2-E7730CF081DD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3698,7 +3856,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000010-D463-402B-B436-56C38C4611DA}"/>
+              <c16:uniqueId val="{00000003-5211-4943-A1D2-E7730CF081DD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3820,7 +3978,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000012-D463-402B-B436-56C38C4611DA}"/>
+              <c16:uniqueId val="{00000005-5211-4943-A1D2-E7730CF081DD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3942,7 +4100,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000014-D463-402B-B436-56C38C4611DA}"/>
+              <c16:uniqueId val="{00000007-5211-4943-A1D2-E7730CF081DD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4064,7 +4222,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000016-D463-402B-B436-56C38C4611DA}"/>
+              <c16:uniqueId val="{00000009-5211-4943-A1D2-E7730CF081DD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4170,7 +4328,7 @@
         <c:axId val="1455861919"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="8000"/>
+          <c:min val="7000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4271,6 +4429,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -4297,6 +4486,7 @@
         <c14:dropZoneFilter val="1"/>
         <c14:dropZoneCategories val="1"/>
         <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
         <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
@@ -4348,12 +4538,9 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Evolução</a:t>
+              <a:t>Evolução do Forecast</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> do Forecast</a:t>
-            </a:r>
+            <a:endParaRPr lang="en-US" baseline="0"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -4496,6 +4683,9 @@
       <c:pivotFmt>
         <c:idx val="5"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -4518,6 +4708,9 @@
       <c:pivotFmt>
         <c:idx val="6"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -4540,6 +4733,9 @@
       <c:pivotFmt>
         <c:idx val="7"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -4562,6 +4758,9 @@
       <c:pivotFmt>
         <c:idx val="8"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -4584,6 +4783,9 @@
       <c:pivotFmt>
         <c:idx val="9"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -4630,7 +4832,7 @@
         <c:spPr>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -4652,7 +4854,7 @@
         <c:spPr>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -4674,6 +4876,116 @@
         <c:spPr>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="14"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="15"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="16"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="17"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="18"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
               <a:schemeClr val="accent4"/>
             </a:solidFill>
             <a:round/>
@@ -4692,7 +5004,7 @@
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="14"/>
+        <c:idx val="19"/>
         <c:spPr>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
@@ -4837,7 +5149,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-79CD-401B-BE94-69ACFDA3A79A}"/>
+              <c16:uniqueId val="{00000001-F81B-4FDE-A3E7-E62C03EB36B6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4959,7 +5271,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-79CD-401B-BE94-69ACFDA3A79A}"/>
+              <c16:uniqueId val="{00000003-F81B-4FDE-A3E7-E62C03EB36B6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5081,7 +5393,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-79CD-401B-BE94-69ACFDA3A79A}"/>
+              <c16:uniqueId val="{00000005-F81B-4FDE-A3E7-E62C03EB36B6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5203,7 +5515,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000D-79CD-401B-BE94-69ACFDA3A79A}"/>
+              <c16:uniqueId val="{00000007-F81B-4FDE-A3E7-E62C03EB36B6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5325,7 +5637,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000F-79CD-401B-BE94-69ACFDA3A79A}"/>
+              <c16:uniqueId val="{00000009-F81B-4FDE-A3E7-E62C03EB36B6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5532,6 +5844,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -5558,6 +5901,7 @@
         <c14:dropZoneFilter val="1"/>
         <c14:dropZoneCategories val="1"/>
         <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
         <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
@@ -6715,15 +7059,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>206375</xdr:colOff>
+      <xdr:colOff>206374</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>126999</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>765175</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6761,10 +7105,10 @@
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>201706</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6802,10 +7146,10 @@
       <xdr:rowOff>120650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>616857</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>99786</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9458,7 +9802,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9FEC6F2F-2A7E-4410-8A16-0BCFF6FE0469}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" rowHeaderCaption="Mês">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9FEC6F2F-2A7E-4410-8A16-0BCFF6FE0469}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13" rowHeaderCaption="Mês">
   <location ref="A3:F16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField numFmtId="164" showAll="0">
@@ -9963,7 +10307,7 @@
       </pivotArea>
     </format>
   </formats>
-  <chartFormats count="20">
+  <chartFormats count="30">
     <chartFormat chart="2" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -10193,6 +10537,126 @@
       </pivotArea>
     </chartFormat>
     <chartFormat chart="8" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="11" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="11" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="11" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="11" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="11" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="12" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="12" format="11" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="12" format="12" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="12" format="13" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="12" format="14" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -10831,7 +11295,7 @@
     </format>
   </formats>
   <chartFormats count="5">
-    <chartFormat chart="0" format="10" series="1">
+    <chartFormat chart="0" format="15" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -10843,7 +11307,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="11" series="1">
+    <chartFormat chart="0" format="16" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -10855,7 +11319,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="12" series="1">
+    <chartFormat chart="0" format="17" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -10867,7 +11331,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="13" series="1">
+    <chartFormat chart="0" format="18" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -10879,7 +11343,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="14" series="1">
+    <chartFormat chart="0" format="19" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -11038,7 +11502,7 @@
     </format>
   </formats>
   <chartFormats count="5">
-    <chartFormat chart="7" format="10" series="1">
+    <chartFormat chart="7" format="15" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -11050,7 +11514,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="7" format="11" series="1">
+    <chartFormat chart="7" format="16" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -11062,7 +11526,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="7" format="12" series="1">
+    <chartFormat chart="7" format="17" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -11074,7 +11538,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="7" format="13" series="1">
+    <chartFormat chart="7" format="18" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -11086,7 +11550,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="7" format="14" series="1">
+    <chartFormat chart="7" format="19" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -13757,7 +14221,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F13DC151-2F51-456C-BC01-B22829A32821}">
   <dimension ref="A3:D8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -13978,7 +14442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB6DBA7E-A9FF-4A72-AA6F-C469452FAD5A}">
   <dimension ref="A3:F16"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -14267,7 +14731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF28296A-4724-4760-BF53-D248BF8B5957}">
   <dimension ref="A3:F16"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -14568,7 +15032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1DCF0F6-38E2-4975-89A4-7577619F8EA9}">
   <dimension ref="A3:F16"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>